<commit_message>
added two mean centers to file
</commit_message>
<xml_diff>
--- a/data/mean_center_range_subsetofprecluded_with_partnerdata.xlsx
+++ b/data/mean_center_range_subsetofprecluded_with_partnerdata.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/annabellestanley/Desktop/RFF/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/usr/local/bin/store/partner_rff/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADC752E6-6A02-6543-B5A0-6E3B85A58A65}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C141A583-7D69-524A-AF0F-2457658CD17A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="460" windowWidth="24640" windowHeight="13760" xr2:uid="{514CAA40-9BC7-6446-B707-3502F5E2042B}"/>
+    <workbookView xWindow="180" yWindow="560" windowWidth="24640" windowHeight="13760" xr2:uid="{514CAA40-9BC7-6446-B707-3502F5E2042B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="118">
   <si>
     <t>Calochortus persistens</t>
   </si>
@@ -373,6 +373,12 @@
   </si>
   <si>
     <t>EAGLE LAKE TROUT</t>
+  </si>
+  <si>
+    <t>Chorizanthe parryi var fernandina</t>
+  </si>
+  <si>
+    <t>San Fernando Valley spineflower</t>
   </si>
 </sst>
 </file>
@@ -735,10 +741,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F9B9175-BF4C-7842-9815-86DA28EA20C5}">
-  <dimension ref="A1:I56"/>
+  <dimension ref="A1:H57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -746,1114 +752,1146 @@
     <col min="1" max="1" width="43.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>112</v>
       </c>
       <c r="B1" t="s">
         <v>113</v>
       </c>
+      <c r="C1" t="s">
+        <v>108</v>
+      </c>
       <c r="D1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="E1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="F1" t="s">
-        <v>110</v>
-      </c>
-      <c r="G1" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>104</v>
       </c>
       <c r="B2" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C2">
+        <v>-12345755.610615199</v>
+      </c>
+      <c r="D2">
+        <v>4625378.7762936596</v>
+      </c>
+      <c r="E2">
+        <v>-110.9038095902</v>
+      </c>
+      <c r="F2">
+        <v>38.324570682198598</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
       </c>
+      <c r="C3">
+        <v>-12060178.1351375</v>
+      </c>
       <c r="D3">
-        <v>-12060178.1351375</v>
+        <v>4048999.8391439202</v>
       </c>
       <c r="E3">
-        <v>4048999.8391439202</v>
+        <v>-108.338423479981</v>
       </c>
       <c r="F3">
-        <v>-108.338423479981</v>
-      </c>
-      <c r="G3">
         <v>34.150287334371498</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>64</v>
       </c>
       <c r="B4" t="s">
         <v>65</v>
       </c>
+      <c r="C4">
+        <v>-13070398.975346699</v>
+      </c>
       <c r="D4">
-        <v>-13070398.975346699</v>
+        <v>4371780.0119410399</v>
       </c>
       <c r="E4">
-        <v>4371780.0119410399</v>
+        <v>-117.413391690941</v>
       </c>
       <c r="F4">
-        <v>-117.413391690941</v>
-      </c>
-      <c r="G4">
         <v>36.5154481590708</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>46</v>
       </c>
       <c r="B5" t="s">
         <v>47</v>
       </c>
+      <c r="C5">
+        <v>-12691940.973887101</v>
+      </c>
       <c r="D5">
-        <v>-12691940.973887101</v>
+        <v>5109426.8165969197</v>
       </c>
       <c r="E5">
-        <v>5109426.8165969197</v>
+        <v>-114.01364561985601</v>
       </c>
       <c r="F5">
-        <v>-114.01364561985601</v>
-      </c>
-      <c r="G5">
         <v>41.654915561413802</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6" t="s">
         <v>5</v>
       </c>
+      <c r="C6">
+        <v>-12977513.5731954</v>
+      </c>
       <c r="D6">
-        <v>-12977513.5731954</v>
+        <v>5470823.7915824996</v>
       </c>
       <c r="E6">
-        <v>5470823.7915824996</v>
+        <v>-116.57898792669999</v>
       </c>
       <c r="F6">
-        <v>-116.57898792669999</v>
-      </c>
-      <c r="G6">
         <v>44.034765434736599</v>
       </c>
+      <c r="G6" s="1"/>
       <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>25</v>
       </c>
       <c r="B7" t="s">
         <v>26</v>
       </c>
+      <c r="C7">
+        <v>-12884474.004484</v>
+      </c>
       <c r="D7">
-        <v>-12884474.004484</v>
+        <v>4458957.6594512602</v>
       </c>
       <c r="E7">
-        <v>4458957.6594512602</v>
+        <v>-115.74319926068701</v>
       </c>
       <c r="F7">
-        <v>-115.74319926068701</v>
-      </c>
-      <c r="G7">
         <v>37.142281976210597</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>0</v>
       </c>
       <c r="B8" t="s">
         <v>1</v>
       </c>
+      <c r="C8">
+        <v>-13685344.064534999</v>
+      </c>
       <c r="D8">
-        <v>-13685344.064534999</v>
+        <v>5104895.8814649098</v>
       </c>
       <c r="E8">
-        <v>5104895.8814649098</v>
+        <v>-122.93753741606299</v>
       </c>
       <c r="F8">
-        <v>-122.93753741606299</v>
-      </c>
-      <c r="G8">
         <v>41.624497357134501</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>92</v>
       </c>
       <c r="B9" t="s">
         <v>93</v>
       </c>
+      <c r="C9">
+        <v>-13709527.124707799</v>
+      </c>
       <c r="D9">
-        <v>-13709527.124707799</v>
+        <v>5266018.0967069203</v>
       </c>
       <c r="E9">
-        <v>5266018.0967069203</v>
+        <v>-123.154777541762</v>
       </c>
       <c r="F9">
-        <v>-123.154777541762</v>
-      </c>
-      <c r="G9">
         <v>42.697348637884097</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>24</v>
       </c>
       <c r="B10" t="s">
         <v>114</v>
       </c>
+      <c r="C10">
+        <v>-12645884.6264497</v>
+      </c>
       <c r="D10">
-        <v>-12645884.6264497</v>
+        <v>5203707.63193643</v>
       </c>
       <c r="E10">
-        <v>5203707.63193643</v>
+        <v>-113.59991441151899</v>
       </c>
       <c r="F10">
-        <v>-113.59991441151899</v>
-      </c>
-      <c r="G10">
         <v>42.284604596388903</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>116</v>
+      </c>
+      <c r="B11" t="s">
+        <v>117</v>
+      </c>
+      <c r="C11">
+        <v>-13214248.398556899</v>
+      </c>
+      <c r="D11">
+        <v>4114646.2528519598</v>
+      </c>
+      <c r="E11">
+        <v>-118.705613045756</v>
+      </c>
+      <c r="F11">
+        <v>34.636900887268602</v>
+      </c>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>29</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B12" t="s">
         <v>30</v>
       </c>
-      <c r="D11">
+      <c r="C12">
         <v>-12455270.5124796</v>
       </c>
-      <c r="E11">
+      <c r="D12">
         <v>4478987.3328285096</v>
       </c>
-      <c r="F11">
+      <c r="E12">
         <v>-111.88759869203599</v>
       </c>
-      <c r="G11">
+      <c r="F12">
         <v>37.285574769617298</v>
       </c>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
         <v>8</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B13" t="s">
         <v>9</v>
       </c>
-      <c r="D12">
+      <c r="C13">
         <v>-12388961.6248373</v>
       </c>
-      <c r="E12">
+      <c r="D13">
         <v>4140879.4628826398</v>
       </c>
-      <c r="F12">
+      <c r="E13">
         <v>-111.291935819616</v>
       </c>
-      <c r="G12">
+      <c r="F13">
         <v>34.830565633464801</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
         <v>62</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B14" t="s">
         <v>63</v>
       </c>
-      <c r="D13">
+      <c r="C14">
         <v>-13347799.7076825</v>
       </c>
-      <c r="E13">
+      <c r="D14">
         <v>4520544.5568132102</v>
       </c>
-      <c r="F13">
+      <c r="E14">
         <v>-119.905324867773</v>
       </c>
-      <c r="G13">
+      <c r="F14">
         <v>37.582007086094997</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
         <v>42</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B15" t="s">
         <v>43</v>
       </c>
-      <c r="D14">
+      <c r="C15">
         <v>-12339382.816178801</v>
       </c>
-      <c r="E14">
+      <c r="D15">
         <v>3701277.5199360098</v>
       </c>
-      <c r="F14">
+      <c r="E15">
         <v>-110.846561803752</v>
       </c>
-      <c r="G14">
+      <c r="F15">
         <v>31.526208233670999</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
         <v>33</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B16" t="s">
         <v>34</v>
       </c>
-      <c r="D15">
+      <c r="C16">
         <v>-12998817.251421699</v>
       </c>
-      <c r="E15">
+      <c r="D16">
         <v>3899193.0566602298</v>
       </c>
-      <c r="F15">
+      <c r="E16">
         <v>-116.770362124286</v>
       </c>
-      <c r="G15">
+      <c r="F16">
         <v>33.029295196735802</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
         <v>78</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B17" t="s">
         <v>79</v>
       </c>
-      <c r="D16">
+      <c r="C17">
         <v>-12998817.251421699</v>
       </c>
-      <c r="E16">
+      <c r="D17">
         <v>3899193.0566602298</v>
       </c>
-      <c r="F16">
+      <c r="E17">
         <v>-116.770362124286</v>
       </c>
-      <c r="G16">
+      <c r="F17">
         <v>33.029295196735802</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+      <c r="H17" s="3"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
         <v>12</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B18" t="s">
         <v>13</v>
       </c>
-      <c r="D17">
+      <c r="C18">
         <v>-13437351.740239199</v>
       </c>
-      <c r="E17">
+      <c r="D18">
         <v>5908370.2913343599</v>
       </c>
-      <c r="F17">
+      <c r="E18">
         <v>-120.70978446347</v>
       </c>
-      <c r="G17">
+      <c r="F18">
         <v>46.793114871121404</v>
       </c>
-      <c r="I17" s="3"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+      <c r="H18" s="3"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
         <v>76</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B19" t="s">
         <v>77</v>
       </c>
-      <c r="D18">
+      <c r="C19">
         <v>-11771138.502324199</v>
       </c>
-      <c r="E18">
+      <c r="D19">
         <v>3844414.4014965701</v>
       </c>
-      <c r="F18">
+      <c r="E19">
         <v>-105.741936281257</v>
       </c>
-      <c r="G18">
+      <c r="F19">
         <v>32.615771464771299</v>
       </c>
-      <c r="I18" s="3"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+      <c r="H19" s="3"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
         <v>20</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B20" t="s">
         <v>21</v>
       </c>
-      <c r="D19">
+      <c r="C20">
         <v>-9906582.1368171908</v>
       </c>
-      <c r="E19">
+      <c r="D20">
         <v>3655158.9191683298</v>
       </c>
-      <c r="F19">
+      <c r="E20">
         <v>-88.992341468883097</v>
       </c>
-      <c r="G19">
+      <c r="F20">
         <v>31.172400431711399</v>
       </c>
-      <c r="I19" s="3"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
         <v>31</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B21" t="s">
         <v>32</v>
       </c>
-      <c r="D20">
+      <c r="C21">
         <v>-13380003.8356227</v>
       </c>
-      <c r="E20">
+      <c r="D21">
         <v>5032493.5979591804</v>
       </c>
-      <c r="F20">
+      <c r="E21">
         <v>-120.19461947117701</v>
       </c>
-      <c r="G20">
+      <c r="F21">
         <v>41.136481862884203</v>
       </c>
-      <c r="H20" s="2"/>
-      <c r="I20" s="2"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
         <v>68</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B22" t="s">
         <v>69</v>
       </c>
-      <c r="D21">
+      <c r="C22">
         <v>-12998817</v>
       </c>
-      <c r="E21">
+      <c r="D22">
         <v>3899193.06</v>
       </c>
-      <c r="F21">
+      <c r="E22">
         <v>-116.77036</v>
       </c>
-      <c r="G21">
+      <c r="F22">
         <v>33.0292952</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
         <v>52</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B23" t="s">
         <v>53</v>
       </c>
-      <c r="D22">
+      <c r="C23">
         <v>-13651592.0914244</v>
       </c>
-      <c r="E22">
+      <c r="D23">
         <v>5163263.7726614196</v>
       </c>
-      <c r="F22">
+      <c r="E23">
         <v>-122.634338282917</v>
       </c>
-      <c r="G22">
+      <c r="F23">
         <v>42.015247856049498</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
         <v>56</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B24" t="s">
         <v>57</v>
       </c>
-      <c r="D23">
+      <c r="C24">
         <v>-12510594.327418</v>
       </c>
-      <c r="E23">
+      <c r="D24">
         <v>4956269.7301983098</v>
       </c>
-      <c r="F23">
+      <c r="E24">
         <v>-112.38458097738599</v>
       </c>
-      <c r="G23">
+      <c r="F24">
         <v>40.618755134351701</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
         <v>82</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B25" t="s">
         <v>83</v>
       </c>
-      <c r="D24">
+      <c r="C25">
         <v>-12915096.6153032</v>
       </c>
-      <c r="E24">
+      <c r="D25">
         <v>5378019.0914684497</v>
       </c>
-      <c r="F24">
+      <c r="E25">
         <v>-116.018286854072</v>
       </c>
-      <c r="G24">
+      <c r="F25">
         <v>43.432388542424903</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
         <v>72</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B26" t="s">
         <v>73</v>
       </c>
-      <c r="D25">
+      <c r="C26">
         <v>-12733244.0639528</v>
       </c>
-      <c r="E25">
+      <c r="D26">
         <v>4296145.0031300001</v>
       </c>
-      <c r="F25">
+      <c r="E26">
         <v>-114.38467759073001</v>
       </c>
-      <c r="G25">
+      <c r="F26">
         <v>35.967461175228202</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
         <v>10</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B27" t="s">
         <v>11</v>
       </c>
-      <c r="D26">
+      <c r="C27">
         <v>-13662053.0653142</v>
       </c>
-      <c r="E26">
+      <c r="D27">
         <v>5226167.3272868898</v>
       </c>
-      <c r="F26">
+      <c r="E27">
         <v>-122.72831081023701</v>
       </c>
-      <c r="G26">
+      <c r="F27">
         <v>42.433691367538401</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
         <v>80</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B28" t="s">
         <v>81</v>
       </c>
-      <c r="D27">
+      <c r="C28">
         <v>-9315092.4319196492</v>
       </c>
-      <c r="E27">
+      <c r="D28">
         <v>4187323.03645337</v>
       </c>
-      <c r="F27">
+      <c r="E28">
         <v>-83.678899045795006</v>
       </c>
-      <c r="G27">
+      <c r="F28">
         <v>35.172316805450798</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
         <v>27</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B29" t="s">
         <v>28</v>
       </c>
-      <c r="D28">
+      <c r="C29">
         <v>-9472967.6486399807</v>
       </c>
-      <c r="E28">
+      <c r="D29">
         <v>5105948.4827497201</v>
       </c>
-      <c r="F28">
+      <c r="E29">
         <v>-85.097116247430606</v>
       </c>
-      <c r="G28">
+      <c r="F29">
         <v>41.631565223019997</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
         <v>98</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B30" t="s">
         <v>99</v>
       </c>
-      <c r="D29">
+      <c r="C30">
         <v>-17312734.0272993</v>
       </c>
-      <c r="E29">
+      <c r="D30">
         <v>2226103.15576438</v>
       </c>
-      <c r="F29">
+      <c r="E30">
         <v>-155.52293586619101</v>
       </c>
-      <c r="G29">
+      <c r="F30">
         <v>19.6033681173652</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
         <v>74</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B31" t="s">
         <v>75</v>
       </c>
-      <c r="D30">
+      <c r="C31">
         <v>-11818227.89776</v>
       </c>
-      <c r="E30">
+      <c r="D31">
         <v>4343466.4178255303</v>
       </c>
-      <c r="F30">
+      <c r="E31">
         <v>-106.164947517656</v>
       </c>
-      <c r="G30">
+      <c r="F31">
         <v>36.310761924800801</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
         <v>37</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B32" t="s">
         <v>115</v>
       </c>
-      <c r="D31">
+      <c r="C32">
         <v>-13424562.069307201</v>
       </c>
-      <c r="E31">
+      <c r="D32">
         <v>4964653.5852393098</v>
       </c>
-      <c r="F31">
+      <c r="E32">
         <v>-120.594892894699</v>
       </c>
-      <c r="G31">
+      <c r="F32">
         <v>40.675897967407899</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
         <v>60</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B33" t="s">
         <v>61</v>
       </c>
-      <c r="D32">
+      <c r="C33">
         <v>-13613287.131936399</v>
       </c>
-      <c r="E32">
+      <c r="D33">
         <v>5039048.0310511803</v>
       </c>
-      <c r="F32">
+      <c r="E33">
         <v>-122.290238977261</v>
       </c>
-      <c r="G32">
+      <c r="F33">
         <v>41.180811634657204</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
         <v>16</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B34" t="s">
         <v>17</v>
       </c>
-      <c r="D33">
+      <c r="C34">
         <v>-12733244.0639528</v>
       </c>
-      <c r="E33">
+      <c r="D34">
         <v>4296145.0031300001</v>
       </c>
-      <c r="F33">
+      <c r="E34">
         <v>-114.38467759073001</v>
       </c>
-      <c r="G33">
+      <c r="F34">
         <v>35.967461175228202</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
         <v>54</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B35" t="s">
         <v>55</v>
       </c>
-      <c r="D34">
+      <c r="C35">
         <v>-12442329.175785</v>
       </c>
-      <c r="E34">
+      <c r="D35">
         <v>4279567.2668158598</v>
       </c>
-      <c r="F34">
+      <c r="E35">
         <v>-111.77134468654</v>
       </c>
-      <c r="G34">
+      <c r="F35">
         <v>35.846840444375097</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
         <v>48</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B36" t="s">
         <v>49</v>
       </c>
-      <c r="D35">
+      <c r="C36">
         <v>-12210343.388276801</v>
       </c>
-      <c r="E35">
+      <c r="D36">
         <v>4868067.10853195</v>
       </c>
-      <c r="F35">
+      <c r="E36">
         <v>-109.68738090036901</v>
       </c>
-      <c r="G35">
+      <c r="F36">
         <v>40.014620433259502</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
         <v>102</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B37" t="s">
         <v>103</v>
       </c>
-      <c r="D36">
+      <c r="C37">
         <v>-12119105.2422408</v>
       </c>
-      <c r="E36">
+      <c r="D37">
         <v>4873829.9541611997</v>
       </c>
-      <c r="F36">
+      <c r="E37">
         <v>-108.86777468958</v>
       </c>
-      <c r="G36">
+      <c r="F37">
         <v>40.054257412239799</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
         <v>18</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B38" t="s">
         <v>19</v>
       </c>
-      <c r="D37">
+      <c r="C38">
         <v>-13081766.560808299</v>
       </c>
-      <c r="E37">
+      <c r="D38">
         <v>3977572.9017163902</v>
       </c>
-      <c r="F37">
+      <c r="E38">
         <v>-117.515508448578</v>
       </c>
-      <c r="G37">
+      <c r="F38">
         <v>33.617622453444604</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
         <v>40</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B39" t="s">
         <v>41</v>
       </c>
-      <c r="D38">
+      <c r="C39">
         <v>-12679909.6642628</v>
       </c>
-      <c r="E38">
+      <c r="D39">
         <v>3864992.33287693</v>
       </c>
-      <c r="F38">
+      <c r="E39">
         <v>-113.905566526621</v>
       </c>
-      <c r="G38">
+      <c r="F39">
         <v>32.771339834520603</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
         <v>84</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B40" t="s">
         <v>85</v>
       </c>
-      <c r="D39">
+      <c r="C40">
         <v>-13286392.631447</v>
       </c>
-      <c r="E39">
+      <c r="D40">
         <v>5018802.4952929504</v>
       </c>
-      <c r="F39">
+      <c r="E40">
         <v>-119.353695716419</v>
       </c>
-      <c r="G39">
+      <c r="F40">
         <v>41.043787759097803</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
         <v>58</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B41" t="s">
         <v>59</v>
       </c>
-      <c r="D40">
+      <c r="C41">
         <v>-9381785.8890246395</v>
       </c>
-      <c r="E40">
+      <c r="D41">
         <v>4539998.4268720597</v>
       </c>
-      <c r="F40">
+      <c r="E41">
         <v>-84.2780165644769</v>
       </c>
-      <c r="G40">
+      <c r="F41">
         <v>37.720369926618702</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
         <v>88</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B42" t="s">
         <v>89</v>
       </c>
-      <c r="D41">
+      <c r="C42">
         <v>-9600044.2392875105</v>
       </c>
-      <c r="E41">
+      <c r="D42">
         <v>4468270.0636078697</v>
       </c>
-      <c r="F41">
+      <c r="E42">
         <v>-86.238664683755403</v>
       </c>
-      <c r="G41">
+      <c r="F42">
         <v>37.208937003747998</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
         <v>14</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B43" t="s">
         <v>15</v>
       </c>
-      <c r="D42">
+      <c r="C43">
         <v>-9387726.0525240898</v>
       </c>
-      <c r="E42">
+      <c r="D43">
         <v>4642044.3702961998</v>
       </c>
-      <c r="F42">
+      <c r="E43">
         <v>-84.331377961094105</v>
       </c>
-      <c r="G42">
+      <c r="F43">
         <v>38.441924237379098</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
         <v>50</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B44" t="s">
         <v>51</v>
       </c>
-      <c r="D43">
+      <c r="C44">
         <v>-9381785.8890246395</v>
       </c>
-      <c r="E43">
+      <c r="D44">
         <v>4539998.4268720597</v>
       </c>
-      <c r="F43">
+      <c r="E44">
         <v>-84.2780165644769</v>
       </c>
-      <c r="G43">
+      <c r="F44">
         <v>37.720369926618702</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
         <v>70</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B45" t="s">
         <v>71</v>
       </c>
-      <c r="D44">
+      <c r="C45">
         <v>-12529512.924317099</v>
       </c>
-      <c r="E44">
+      <c r="D45">
         <v>4109991.19950108</v>
       </c>
-      <c r="F44">
+      <c r="E45">
         <v>-112.55452962487099</v>
       </c>
-      <c r="G44">
+      <c r="F45">
         <v>34.602487913021399</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
         <v>38</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B46" t="s">
         <v>39</v>
       </c>
-      <c r="D45">
+      <c r="C46">
         <v>-13148223.1935868</v>
       </c>
-      <c r="E45">
+      <c r="D46">
         <v>5072951.4053465901</v>
       </c>
-      <c r="F45">
+      <c r="E46">
         <v>-118.112498538138</v>
       </c>
-      <c r="G45">
+      <c r="F46">
         <v>41.409632407954</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
         <v>90</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B47" t="s">
         <v>91</v>
       </c>
-      <c r="D46">
+      <c r="C47">
         <v>-13364341.1837059</v>
       </c>
-      <c r="E46">
+      <c r="D47">
         <v>4767697.76676015</v>
       </c>
-      <c r="F46">
+      <c r="E47">
         <v>-120.053919475111</v>
       </c>
-      <c r="G46">
+      <c r="F47">
         <v>39.320588851797297</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
         <v>35</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B48" t="s">
         <v>36</v>
       </c>
-      <c r="D47">
+      <c r="C48">
         <v>-11488766.646066699</v>
       </c>
-      <c r="E47">
+      <c r="D48">
         <v>3850854.3053644001</v>
       </c>
-      <c r="F47">
+      <c r="E48">
         <v>-103.205346738443</v>
       </c>
-      <c r="G47">
+      <c r="F48">
         <v>32.664486031527197</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
         <v>106</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B49" t="s">
         <v>107</v>
       </c>
-      <c r="D48">
+      <c r="C49">
         <v>-8914268.6486863308</v>
       </c>
-      <c r="E48">
+      <c r="D49">
         <v>4207779.2440125998</v>
       </c>
-      <c r="F48">
+      <c r="E49">
         <v>-80.078237738624097</v>
       </c>
-      <c r="G48">
+      <c r="F49">
         <v>35.322388683770598</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
         <v>100</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B50" t="s">
         <v>101</v>
       </c>
-      <c r="D49">
+      <c r="C50">
         <v>-12232628.0045397</v>
       </c>
-      <c r="E49">
+      <c r="D50">
         <v>3886603.6464946601</v>
       </c>
-      <c r="F49">
+      <c r="E50">
         <v>-109.887567014265</v>
       </c>
-      <c r="G49">
+      <c r="F50">
         <v>32.934428290831399</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
         <v>66</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B51" t="s">
         <v>67</v>
       </c>
-      <c r="D50">
+      <c r="C51">
         <v>-8056909.8220941396</v>
       </c>
-      <c r="E50">
+      <c r="D51">
         <v>5255952.1820408497</v>
       </c>
-      <c r="F50">
+      <c r="E51">
         <v>-72.376452359598602</v>
       </c>
-      <c r="G50">
+      <c r="F51">
         <v>42.630856581193697</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
         <v>44</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B52" t="s">
         <v>45</v>
       </c>
-      <c r="D51">
+      <c r="C52">
         <v>-9285513.4083641209</v>
       </c>
-      <c r="E51">
+      <c r="D52">
         <v>4047675.5990346801</v>
       </c>
-      <c r="F51">
+      <c r="E52">
         <v>-83.413186156302402</v>
       </c>
-      <c r="G51">
+      <c r="F52">
         <v>34.140442135368197</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A52" t="s">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
         <v>22</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B53" t="s">
         <v>23</v>
       </c>
-      <c r="D52">
+      <c r="C53">
         <v>-12803246.9288757</v>
       </c>
-      <c r="E52">
+      <c r="D53">
         <v>4330759.6497030202</v>
       </c>
-      <c r="F52">
+      <c r="E53">
         <v>-115.01352402565399</v>
       </c>
-      <c r="G52">
+      <c r="F53">
         <v>36.2187262140027</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
         <v>6</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B54" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
         <v>86</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B55" t="s">
         <v>87</v>
       </c>
-      <c r="D54">
+      <c r="C55">
         <v>-12979768.9382114</v>
       </c>
-      <c r="E54">
+      <c r="D55">
         <v>5520460.8689932302</v>
       </c>
-      <c r="F54">
+      <c r="E55">
         <v>-116.59924821535201</v>
       </c>
-      <c r="G54">
+      <c r="F55">
         <v>44.354462072097299</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A55" t="s">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
         <v>96</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B56" t="s">
         <v>97</v>
       </c>
-      <c r="D55">
+      <c r="C56">
         <v>-13255971.6300977</v>
       </c>
-      <c r="E55">
+      <c r="D56">
         <v>5940184.6543896804</v>
       </c>
-      <c r="F55">
+      <c r="E56">
         <v>-119.08041921171601</v>
       </c>
-      <c r="G55">
+      <c r="F56">
         <v>46.988423234922799</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A56" t="s">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
         <v>94</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B57" t="s">
         <v>95</v>
       </c>
-      <c r="D56">
+      <c r="C57">
         <v>-12375413.148993701</v>
       </c>
-      <c r="E56">
+      <c r="D57">
         <v>5707815.4704382401</v>
       </c>
-      <c r="F56">
+      <c r="E57">
         <v>-111.17022779034799</v>
       </c>
-      <c r="G56">
+      <c r="F57">
         <v>45.545521614663897</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:B56">
-    <sortCondition ref="A3"/>
+  <sortState ref="A2:F57">
+    <sortCondition ref="A2"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>